<commit_message>
Week menu update finalize
</commit_message>
<xml_diff>
--- a/Weekly menu.xlsx
+++ b/Weekly menu.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nandi\Google Drive\recipies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/TranscendCard/sourcetree/nandini_recipies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7459BDBE-B34D-4AA7-BF6E-53C343D91D77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E228C79-E47B-FB42-9ED9-4EC6983E8615}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2F3F79CF-486F-4E95-9DB8-B59FBA73AE39}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" xr2:uid="{2F3F79CF-486F-4E95-9DB8-B59FBA73AE39}"/>
   </bookViews>
   <sheets>
     <sheet name="Weekly schedule" sheetId="3" r:id="rId1"/>
+    <sheet name="Amit Things to consider next" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>arbi</t>
   </si>
@@ -71,24 +72,10 @@
     <t>Coconut rice</t>
   </si>
   <si>
-    <t>Rice special</t>
-  </si>
-  <si>
-    <t>South indian special</t>
-  </si>
-  <si>
     <t>curd rice</t>
   </si>
   <si>
-    <t>Sunday special</t>
-  </si>
-  <si>
     <t>chana dal/chilka moong dal/palak paneer</t>
-  </si>
-  <si>
-    <t>Fried idli
-Nariyal chutney
-Sambhar</t>
   </si>
   <si>
     <t>Plain idli
@@ -97,6 +84,109 @@
 cheela</t>
   </si>
   <si>
+    <t>Beetroot subji
+Sabut moong dal
+Roti</t>
+  </si>
+  <si>
+    <t>Aloo Shimla mirch ki subji
+yellow moong dal
+roti</t>
+  </si>
+  <si>
+    <t>1- Most important. Improve  the recipe which has failed last in last weekend.
+2- Try to adapt recipies according to season if required
+3- If that is done, Try something new.</t>
+  </si>
+  <si>
+    <t>Kaccha kela subji
+Chilka moong dal
+Roti</t>
+  </si>
+  <si>
+    <t>Kundru
+Baigan
+Tur Dal
+kadhi plain/kofta</t>
+  </si>
+  <si>
+    <t>Karela Subji</t>
+  </si>
+  <si>
+    <t>Rajasthani dal dhokli</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Pmqwti9kWj4</t>
+  </si>
+  <si>
+    <t>Lauki kofta</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=soUKwdZS2zA</t>
+  </si>
+  <si>
+    <t>Palak kofta</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=xIa0h2tKMfk</t>
+  </si>
+  <si>
+    <t>Besan stuffed karela</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=wNxu8-EQ-oA</t>
+  </si>
+  <si>
+    <t>Dalia pulav</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=eWZ0UVISyBY</t>
+  </si>
+  <si>
+    <t>Rava Upma</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=SogcWMwjxS0</t>
+  </si>
+  <si>
+    <t>Bharma Karela</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Hvvj-zn-Uwk</t>
+  </si>
+  <si>
+    <t>Sooji cutlets</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=jtXkMrFiRyw</t>
+  </si>
+  <si>
+    <t>Veg manchurian</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=DqKxuiaShkA</t>
+  </si>
+  <si>
+    <t>Khatta meetha chiwda</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=iuetmjAUi4I</t>
+  </si>
+  <si>
+    <t>Chana dal tadka</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=-IJuLjmnt-4</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Fried idli</t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -105,27 +195,28 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Baigan
-snake gourd
-tur dal
+      <t xml:space="preserve">
+Nariyal chutney
 </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>roti</t>
+      <t>Sambhar</t>
     </r>
   </si>
   <si>
-    <t>Kundru
-kadhi plain/kofta</t>
-  </si>
-  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>biryani</t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -134,41 +225,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>kaccha kela
-Palak paneer</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">
-roti</t>
-    </r>
-  </si>
-  <si>
-    <t>Beetroot subji
-Sabut moong dal
-Roti</t>
-  </si>
-  <si>
-    <t>Aloo Shimla mirch ki subji
-yellow moong dal
-roti</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">biryani
 aloo turai tamatar curry
 </t>
     </r>
@@ -190,7 +247,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +269,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -230,10 +300,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -248,8 +319,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -562,24 +638,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D67F1A-23E7-4361-A92D-D3AC17E09FFA}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="27.1640625" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
-    <col min="7" max="7" width="26.5703125" customWidth="1"/>
+    <col min="7" max="7" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -602,80 +678,185 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" ht="96">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="5" customFormat="1" ht="64">
+      <c r="A3" s="4"/>
+      <c r="B3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="32">
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="32">
+      <c r="G5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="16">
+      <c r="G6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="16">
+      <c r="G7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="16">
+      <c r="G8" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EDA7BB1-05D7-714E-BE1A-3523880FE1B4}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{9B25A99F-4A58-B945-AFE4-5B34C725E006}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{1941683B-5AF6-E340-9A38-93F8EDF50B39}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>